<commit_message>
phone is now really hidden before searching for it
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8624437D-EEDD-4B25-AA76-0E6777A0B44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D870A5A8-081E-4489-9161-6BE3619DA765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -88,9 +88,6 @@
     <t>fleshplate doesn't fall down perfectly</t>
   </si>
   <si>
-    <t>hide phone before last quest</t>
-  </si>
-  <si>
     <t>last food too late horror event</t>
   </si>
   <si>
@@ -256,9 +253,6 @@
     <t>water bottle, more glasses in the kitchen</t>
   </si>
   <si>
-    <t>H13 JumpingSpider: lower immersedvalue before so you aren't too close to the screen, fine tuning, reaction, crawling away</t>
-  </si>
-  <si>
     <t>H10 + H15 Flesh Plate: Flesh SFX, small glitch effect with the glitch sound</t>
   </si>
   <si>
@@ -290,6 +284,12 @@
   </si>
   <si>
     <t>"Hello?", "Who's there?", "Weird"</t>
+  </si>
+  <si>
+    <t>Microwave: 3D Audio (Humming), auto stop</t>
+  </si>
+  <si>
+    <t>H13 JumpingSpider: Hide Spider before event, lower immersedvalue before so you aren't too close to the screen, fine tuning, reaction, crawling away, interferance with Looking-For-Phone-Quest</t>
   </si>
 </sst>
 </file>
@@ -652,11 +652,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,74 +679,74 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>32</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -757,13 +757,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -771,94 +771,95 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>11</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>11</v>
       </c>
       <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
         <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10">
-        <v>11</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C11">
-        <v>12</v>
-      </c>
-      <c r="D11">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="C13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>19</v>
@@ -869,10 +870,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>19</v>
@@ -883,10 +884,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16">
         <v>20</v>
@@ -900,7 +901,7 @@
         <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17">
         <v>20</v>
@@ -911,10 +912,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -925,10 +926,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19">
         <v>21</v>
@@ -939,10 +940,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20">
         <v>33</v>
@@ -956,7 +957,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <v>40</v>
@@ -967,10 +968,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22">
         <v>40</v>
@@ -981,10 +982,10 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>40</v>
@@ -995,10 +996,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C24">
         <v>48</v>
@@ -1009,10 +1010,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <v>48</v>
@@ -1023,10 +1024,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26">
         <v>48</v>
@@ -1037,10 +1038,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27">
         <v>49</v>
@@ -1051,10 +1052,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C28">
         <v>49</v>
@@ -1065,10 +1066,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29">
         <v>49</v>
@@ -1079,10 +1080,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>50</v>
@@ -1096,7 +1097,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31">
         <v>50</v>
@@ -1107,10 +1108,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>51</v>
@@ -1119,15 +1120,15 @@
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C33">
         <v>51</v>
@@ -1138,10 +1139,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34">
         <v>60</v>
@@ -1152,10 +1153,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35">
         <v>70</v>
@@ -1166,10 +1167,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36">
         <v>98</v>
@@ -1180,10 +1181,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C37">
         <v>99</v>
@@ -1194,10 +1195,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" t="s">
         <v>63</v>
-      </c>
-      <c r="B38" t="s">
-        <v>64</v>
       </c>
       <c r="C38">
         <v>99</v>
@@ -1208,10 +1209,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C39">
         <v>99</v>
@@ -1225,7 +1226,7 @@
         <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40">
         <v>100</v>
@@ -1236,10 +1237,10 @@
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41">
         <v>100</v>
@@ -1250,10 +1251,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42">
         <v>110</v>
@@ -1267,7 +1268,7 @@
         <v>13</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43">
         <v>110</v>
@@ -1278,10 +1279,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C44">
         <v>120</v>
@@ -1292,10 +1293,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C45">
         <v>199</v>
@@ -1306,10 +1307,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C46">
         <v>200</v>
@@ -1323,7 +1324,7 @@
         <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47">
         <v>999</v>
@@ -1337,7 +1338,7 @@
         <v>6</v>
       </c>
       <c r="B48" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C48">
         <v>1000</v>
@@ -1351,7 +1352,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49">
         <v>1000</v>
@@ -1365,7 +1366,7 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1373,15 +1374,15 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1389,127 +1390,127 @@
         <v>12</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B59" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="B61" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B61" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B64" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,9 +1536,6 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E77" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
added small batches of spiders after H6
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BDE8CB-FE37-476B-A4C4-4BD31601551C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2D72E3-305E-4F1F-A4C5-75F9A41C5AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="84">
   <si>
     <t>Description</t>
   </si>
@@ -268,9 +268,6 @@
     <t>Gameplay Addition, Horror</t>
   </si>
   <si>
-    <t>After H6 SpiderCrawl: Many many batches of spiders here and there (ultra low poly or just a png, should move with a shader)</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>H13 JumpingSpider: lower immersedvalue before so you aren't too close to the screen, fine tuning, reaction, crawling away, interferance with Looking-For-Phone-Quest</t>
+  </si>
+  <si>
+    <t>"Nothing in there", "Locked?"</t>
   </si>
 </sst>
 </file>
@@ -370,10 +370,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E67" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E67">
-    <sortCondition ref="C2:C67"/>
-    <sortCondition ref="D2:D67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E66" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E66">
+    <sortCondition ref="C2:C66"/>
+    <sortCondition ref="D2:D66"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -649,7 +649,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -679,26 +679,29 @@
         <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -712,13 +715,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -726,106 +729,106 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <v>11</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>11</v>
       </c>
       <c r="D6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8">
         <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>30</v>
       </c>
       <c r="C11">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D11">
-        <v>4</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
         <v>30</v>
@@ -839,21 +842,21 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>30</v>
       </c>
       <c r="C13">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
@@ -867,7 +870,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
@@ -876,54 +879,54 @@
         <v>20</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>29</v>
+        <v>62</v>
       </c>
       <c r="C17">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="C18">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D18">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
@@ -935,9 +938,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>30</v>
@@ -949,40 +952,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="C21">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="C22">
         <v>48</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="C23">
         <v>48</v>
@@ -993,21 +996,21 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C24">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
         <v>61</v>
@@ -1021,35 +1024,35 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C26">
         <v>49</v>
       </c>
       <c r="D26">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>29</v>
       </c>
       <c r="C27">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
         <v>29</v>
@@ -1058,29 +1061,32 @@
         <v>50</v>
       </c>
       <c r="D28">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C29">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E29" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C30">
         <v>51</v>
@@ -1088,97 +1094,94 @@
       <c r="D30">
         <v>7</v>
       </c>
-      <c r="E30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C32">
         <v>60</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C33">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D33">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>72</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C34">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D34">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C35">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D35">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="B36" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C36">
         <v>99</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B37" t="s">
         <v>61</v>
@@ -1187,26 +1190,26 @@
         <v>99</v>
       </c>
       <c r="D37">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C38">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D38">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B39" t="s">
         <v>29</v>
@@ -1215,26 +1218,26 @@
         <v>100</v>
       </c>
       <c r="D39">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C40">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D40">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
@@ -1243,82 +1246,82 @@
         <v>110</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="B42" t="s">
         <v>30</v>
       </c>
       <c r="C42">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D42">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="B43" t="s">
-        <v>30</v>
+        <v>74</v>
       </c>
       <c r="C43">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D43">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C44">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D44">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C45">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D45">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>5</v>
+      <c r="A46" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B46" t="s">
         <v>29</v>
       </c>
       <c r="C46">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D46">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>6</v>
+      <c r="A47" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B47" t="s">
         <v>29</v>
@@ -1327,42 +1330,36 @@
         <v>1000</v>
       </c>
       <c r="D47">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C48">
-        <v>1000</v>
-      </c>
-      <c r="D48">
-        <v>9</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
         <v>56</v>
@@ -1370,15 +1367,15 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B53" t="s">
         <v>56</v>
@@ -1386,7 +1383,7 @@
     </row>
     <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
@@ -1394,7 +1391,7 @@
     </row>
     <row r="55" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -1402,47 +1399,47 @@
     </row>
     <row r="56" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B58" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>42</v>
+      <c r="A59" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>43</v>
+      <c r="A60" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B60" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
-        <v>44</v>
+      <c r="A61" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B61" t="s">
         <v>56</v>
@@ -1450,7 +1447,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B62" t="s">
         <v>56</v>
@@ -1458,7 +1455,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B63" t="s">
         <v>56</v>
@@ -1466,7 +1463,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B64" t="s">
         <v>56</v>
@@ -1474,27 +1471,22 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>65</v>
+      <c r="A66" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B66" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" t="s">
-        <v>56</v>
-      </c>
+      <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E68" s="2"/>
@@ -1516,9 +1508,6 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E75" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
added pictures to picture frames
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C45905-6708-465F-9042-3A7410D17B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E9E9DD-5C6C-4D67-8E6D-90A32DD235D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="80">
   <si>
     <t>Description</t>
   </si>
@@ -275,12 +275,6 @@
   </si>
   <si>
     <t>H13 JumpingSpider: lower immersedvalue before so you aren't too close to the screen, fine tuning, reaction, crawling away, interferance with Looking-For-Phone-Quest</t>
-  </si>
-  <si>
-    <t>add paintings</t>
-  </si>
-  <si>
-    <t>This Cat does not exist</t>
   </si>
 </sst>
 </file>
@@ -364,10 +358,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E64" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
-    <sortCondition ref="C3:C64"/>
-    <sortCondition ref="D3:D64"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E63" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E63">
+    <sortCondition ref="C2:C63"/>
+    <sortCondition ref="D2:D63"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -643,11 +637,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,109 +672,106 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C3">
         <v>11</v>
       </c>
       <c r="D3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
       <c r="C8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
@@ -794,21 +785,21 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>28</v>
       </c>
       <c r="C10">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>28</v>
@@ -822,7 +813,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
@@ -831,54 +822,54 @@
         <v>20</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>59</v>
       </c>
       <c r="C14">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C15">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>28</v>
@@ -890,9 +881,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
@@ -904,40 +895,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>72</v>
       </c>
       <c r="C18">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>48</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="C20">
         <v>48</v>
@@ -948,21 +939,21 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C21">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>58</v>
@@ -976,35 +967,35 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C23">
         <v>49</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
       <c r="C24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>27</v>
@@ -1013,29 +1004,32 @@
         <v>50</v>
       </c>
       <c r="D25">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>51</v>
+      </c>
+      <c r="D26">
         <v>7</v>
       </c>
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26">
-        <v>50</v>
-      </c>
-      <c r="D26">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C27">
         <v>51</v>
@@ -1043,97 +1037,94 @@
       <c r="D27">
         <v>7</v>
       </c>
-      <c r="E27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="C28">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D28">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C29">
         <v>60</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D30">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>69</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C31">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D32">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C33">
         <v>99</v>
       </c>
       <c r="D33">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
@@ -1142,26 +1133,26 @@
         <v>99</v>
       </c>
       <c r="D34">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C35">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D35">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
         <v>27</v>
@@ -1170,26 +1161,26 @@
         <v>100</v>
       </c>
       <c r="D36">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C37">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D37">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B38" t="s">
         <v>28</v>
@@ -1198,82 +1189,82 @@
         <v>110</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B39" t="s">
         <v>28</v>
       </c>
       <c r="C39">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D39">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="C40">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D40">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C41">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D41">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="C42">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D42">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>5</v>
+      <c r="A43" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B43" t="s">
         <v>27</v>
       </c>
       <c r="C43">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>6</v>
+      <c r="A44" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B44" t="s">
         <v>27</v>
@@ -1282,174 +1273,163 @@
         <v>1000</v>
       </c>
       <c r="D44">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>27</v>
-      </c>
-      <c r="C45">
-        <v>1000</v>
-      </c>
-      <c r="D45">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B47" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B48" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B53" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>40</v>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
-        <v>41</v>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B57" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>42</v>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B58" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B60" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>62</v>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="B63" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" t="s">
-        <v>53</v>
-      </c>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="2"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="2"/>
@@ -1471,9 +1451,6 @@
     </row>
     <row r="71" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E72" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
fixed staff still charging when player is frozen
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E9E9DD-5C6C-4D67-8E6D-90A32DD235D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB618442-DA99-4232-95AF-450EC8D87981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>Description</t>
   </si>
@@ -94,9 +94,6 @@
     <t>typisches leichtes bassiges beben</t>
   </si>
   <si>
-    <t>charging staff + freeze -&gt; stop charging</t>
-  </si>
-  <si>
     <t>put minigames here and there, e.g. a gameboy with tetris</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>somehow smoothly ground player during freeze (manually enable gravitiy?)</t>
   </si>
   <si>
-    <t>spieler nicht vom pc ausschließen (tasks dafür auch anpassen -&gt; wenn man die vernachl\xE4ssigt, sollen neue horror events den spieler zuerst nerven, dann töten)</t>
-  </si>
-  <si>
     <t>instead of forcing the player to do all tasks sequentially, give him a list of things to do (maybe event do it so that the player isn't blocked from playing)</t>
   </si>
   <si>
@@ -145,9 +139,6 @@
     <t>QoL, SFX Addition</t>
   </si>
   <si>
-    <t>Bugfix</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mutter ruft am Anfang an und sagt, man solle die Tasks machen, die auf einem Zettel stehen, bevor die morgen früh wieder kommt </t>
   </si>
   <si>
@@ -275,6 +266,9 @@
   </si>
   <si>
     <t>H13 JumpingSpider: lower immersedvalue before so you aren't too close to the screen, fine tuning, reaction, crawling away, interferance with Looking-For-Phone-Quest</t>
+  </si>
+  <si>
+    <t>spieler nicht vom pc ausschließen (tasks dafür auch anpassen -&gt; wenn man die vernachlässigt, sollen neue horror events den spieler zuerst nerven, dann töten)</t>
   </si>
 </sst>
 </file>
@@ -337,12 +331,12 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -358,13 +352,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E63" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E63">
-    <sortCondition ref="C2:C63"/>
-    <sortCondition ref="D2:D63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E62" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E62">
+    <sortCondition ref="C2:C62"/>
+    <sortCondition ref="D2:D62"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{FE0B1C3C-98C3-4A53-BB36-B09B8B6E281C}" name="Type"/>
     <tableColumn id="3" xr3:uid="{5DD8EB09-8914-40D5-924D-451D2B02BA4C}" name="Priority"/>
     <tableColumn id="4" xr3:uid="{E0C4F60E-BEC0-48F5-8017-79F3081EDA3C}" name="Est. Workload (0-10)"/>
@@ -637,9 +631,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -664,103 +658,103 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <v>11</v>
       </c>
       <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
         <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="C5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>6</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" s="2"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>19</v>
@@ -771,24 +765,24 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>20</v>
@@ -799,66 +793,66 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C11">
         <v>20</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D12">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C13">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C14">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D14">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15">
         <v>40</v>
@@ -867,12 +861,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>40</v>
@@ -881,40 +875,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C17">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>25</v>
       </c>
       <c r="C18">
         <v>48</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
       <c r="C19">
         <v>48</v>
@@ -925,24 +919,24 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C20">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>49</v>
@@ -953,66 +947,69 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C22">
         <v>49</v>
       </c>
       <c r="D22">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24">
         <v>50</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>51</v>
+      </c>
+      <c r="D25">
         <v>7</v>
       </c>
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25">
-        <v>50</v>
-      </c>
-      <c r="D25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>51</v>
@@ -1020,413 +1017,399 @@
       <c r="D26">
         <v>7</v>
       </c>
-      <c r="E26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>64</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="C27">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D27">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C28">
         <v>60</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C29">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C31">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D31">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C32">
         <v>99</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>99</v>
       </c>
       <c r="D33">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D34">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C35">
         <v>100</v>
       </c>
       <c r="D35">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C37">
         <v>110</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C38">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="C39">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D39">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
       <c r="B40" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="C40">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D40">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C41">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D41">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>5</v>
+      <c r="A42" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B42" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C42">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>6</v>
+      <c r="A43" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C43">
         <v>1000</v>
       </c>
       <c r="D43">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>27</v>
-      </c>
-      <c r="C44">
-        <v>1000</v>
-      </c>
-      <c r="D44">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B50" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B53" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B52" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B53" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="B55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B54" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>42</v>
+      <c r="A57" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B57" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B59" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B60" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" t="s">
-        <v>53</v>
-      </c>
+      <c r="E63" s="2"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E64" s="2"/>
@@ -1449,12 +1432,9 @@
     <row r="70" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E70" s="2"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E71" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Unclear">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Unclear">
       <formula>NOT(ISERROR(SEARCH("Unclear",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added door to a (potential) garden
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307CF1DB-01DD-4080-B16D-EC801B2B3CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DE0F3E-A5A6-4219-9701-351A41AC8175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
   <si>
     <t>Description</t>
   </si>
@@ -88,9 +88,6 @@
     <t>'random rocks, fallen trees on green grass '</t>
   </si>
   <si>
-    <t>gamePlayer death nearestSaveLocation</t>
-  </si>
-  <si>
     <t>typisches leichtes bassiges beben</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t xml:space="preserve">Wäsche zusammenlegen quest </t>
   </si>
   <si>
-    <t>Terrassentür</t>
-  </si>
-  <si>
     <t>The glitch und andere glitches in game haben</t>
   </si>
   <si>
@@ -188,9 +182,6 @@
   </si>
   <si>
     <t>man wird nur ins spiel gezogen, wenn man zu viel spielt</t>
-  </si>
-  <si>
-    <t>Visual Only</t>
   </si>
   <si>
     <t>Straße mit random Autos, manche Autos auffällig langsam, manche bleiben sogar stehen, gleiches mit Passanten</t>
@@ -343,10 +334,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E60" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E60">
-    <sortCondition ref="C2:C60"/>
-    <sortCondition ref="D2:D60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E58" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
+    <sortCondition ref="C2:C58"/>
+    <sortCondition ref="D2:D58"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -622,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -649,106 +640,106 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2">
         <v>4</v>
       </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -756,52 +747,52 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="C9">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="C11">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>40</v>
@@ -812,97 +803,97 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="C13">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C14">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15">
         <v>48</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C16">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="C17">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <v>49</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C19">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -910,72 +901,72 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
         <v>25</v>
       </c>
       <c r="C21">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22">
+        <v>51</v>
+      </c>
+      <c r="D22">
         <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22">
-        <v>50</v>
-      </c>
-      <c r="D22">
-        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23">
+        <v>60</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
         <v>26</v>
       </c>
-      <c r="C23">
-        <v>51</v>
-      </c>
-      <c r="D23">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="C24">
         <v>60</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24">
-        <v>51</v>
       </c>
       <c r="D24">
         <v>7</v>
@@ -983,55 +974,55 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C25">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="D26">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>65</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="D27">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="C28">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D28">
         <v>8</v>
@@ -1039,97 +1030,97 @@
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C29">
         <v>99</v>
       </c>
       <c r="D29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C30">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D30">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C31">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D31">
-        <v>8.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
       </c>
       <c r="C32">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>63</v>
       </c>
       <c r="C35">
-        <v>110</v>
+        <v>199</v>
       </c>
       <c r="D35">
         <v>6</v>
@@ -1137,239 +1128,217 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="C36">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="D36">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="C37">
-        <v>199</v>
+        <v>999</v>
       </c>
       <c r="D37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C38">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="D38">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C39">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>6</v>
+      <c r="A40" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40">
-        <v>1000</v>
-      </c>
-      <c r="D40">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>25</v>
-      </c>
-      <c r="C41">
-        <v>1000</v>
-      </c>
-      <c r="D41">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="B44" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B45" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>37</v>
+      <c r="A52" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>38</v>
+      <c r="A53" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>39</v>
+      <c r="A54" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>42</v>
+      <c r="A58" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B59" t="s">
-        <v>49</v>
-      </c>
+      <c r="E59" s="2"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" t="s">
-        <v>49</v>
-      </c>
+      <c r="E60" s="2"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E61" s="2"/>
@@ -1388,12 +1357,6 @@
     </row>
     <row r="66" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E68" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
microwave now stops automatically after 30s and its audio is now 3D
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4DE0F3E-A5A6-4219-9701-351A41AC8175}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D7926B-60B6-4629-BAD4-E1A3712FA540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -236,9 +236,6 @@
   </si>
   <si>
     <t>"Hello?", "Who's there?", "Weird"</t>
-  </si>
-  <si>
-    <t>Microwave: 3D Audio (Humming), auto stop</t>
   </si>
   <si>
     <t>even more quests</t>
@@ -334,10 +331,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E58" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E58">
-    <sortCondition ref="C2:C58"/>
-    <sortCondition ref="D2:D58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E57" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E57">
+    <sortCondition ref="C2:C57"/>
+    <sortCondition ref="D2:D57"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -613,7 +610,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -648,22 +645,21 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
       <c r="C2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -677,21 +673,21 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>25</v>
       </c>
       <c r="C4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -705,7 +701,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -714,54 +710,54 @@
         <v>20</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D8">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="C9">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -773,9 +769,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -787,40 +783,40 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="C12">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <v>48</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C14">
         <v>48</v>
@@ -831,21 +827,21 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C15">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B16" t="s">
         <v>51</v>
@@ -859,35 +855,35 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C17">
         <v>49</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>24</v>
       </c>
       <c r="C18">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B19" t="s">
         <v>24</v>
@@ -896,29 +892,32 @@
         <v>50</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>51</v>
+      </c>
+      <c r="D20">
         <v>7</v>
       </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20">
-        <v>50</v>
-      </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C21">
         <v>51</v>
@@ -926,97 +925,94 @@
       <c r="D21">
         <v>7</v>
       </c>
-      <c r="E21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="C22">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D22">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C23">
         <v>60</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25">
+        <v>98</v>
+      </c>
+      <c r="D25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
         <v>25</v>
       </c>
-      <c r="C25">
-        <v>70</v>
-      </c>
-      <c r="D25">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
       <c r="C26">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D26">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>99</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" t="s">
         <v>51</v>
@@ -1025,26 +1021,26 @@
         <v>99</v>
       </c>
       <c r="D28">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C29">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D29">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>24</v>
@@ -1053,26 +1049,26 @@
         <v>100</v>
       </c>
       <c r="D30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C31">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D31">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
@@ -1081,82 +1077,82 @@
         <v>110</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D33">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>63</v>
       </c>
       <c r="C34">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D34">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C35">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D35">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="C36">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>5</v>
+      <c r="A37" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B37" t="s">
         <v>24</v>
       </c>
       <c r="C37">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>6</v>
+      <c r="A38" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -1165,42 +1161,36 @@
         <v>1000</v>
       </c>
       <c r="D38">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39">
-        <v>1000</v>
-      </c>
-      <c r="D39">
-        <v>9</v>
+        <v>47</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
@@ -1208,15 +1198,15 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B44" t="s">
         <v>47</v>
@@ -1224,7 +1214,7 @@
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
         <v>47</v>
@@ -1232,7 +1222,7 @@
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B46" t="s">
         <v>47</v>
@@ -1240,47 +1230,47 @@
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>36</v>
+      <c r="A50" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="B50" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>37</v>
+      <c r="A51" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B51" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="4" t="s">
-        <v>38</v>
+      <c r="A52" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B52" t="s">
         <v>47</v>
@@ -1288,7 +1278,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
         <v>47</v>
@@ -1296,7 +1286,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B54" t="s">
         <v>47</v>
@@ -1304,7 +1294,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B55" t="s">
         <v>47</v>
@@ -1312,27 +1302,22 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>55</v>
+      <c r="A57" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B57" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B58" t="s">
-        <v>47</v>
-      </c>
+      <c r="E58" s="2"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E59" s="2"/>
@@ -1354,9 +1339,6 @@
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E66" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
players now still have gravity after being frozen (with exceptions)
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D7926B-60B6-4629-BAD4-E1A3712FA540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975AF580-03A4-4CFE-9275-763FEABEDE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
   <si>
     <t>Description</t>
   </si>
@@ -76,9 +76,6 @@
     <t>dialogue variation in food task</t>
   </si>
   <si>
-    <t>somehow ground player after teleporting</t>
-  </si>
-  <si>
     <t>fleshplate doesn't fall down perfectly</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
   </si>
   <si>
     <t>?? TankBattlePremium Experimental 2 Ending instead of/after current ending</t>
-  </si>
-  <si>
-    <t>somehow smoothly ground player during freeze (manually enable gravitiy?)</t>
   </si>
   <si>
     <t>instead of forcing the player to do all tasks sequentially, give him a list of things to do (maybe event do it so that the player isn't blocked from playing)</t>
@@ -331,10 +325,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E57" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E57">
-    <sortCondition ref="C2:C57"/>
-    <sortCondition ref="D2:D57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E55" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E55">
+    <sortCondition ref="C2:C55"/>
+    <sortCondition ref="D2:D55"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -610,7 +604,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -637,63 +631,63 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
-      </c>
       <c r="D3">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -701,52 +695,52 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C6">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="C8">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>40</v>
@@ -757,97 +751,97 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="C10">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12">
         <v>48</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C13">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="C14">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C15">
         <v>49</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C16">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -855,72 +849,72 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C17">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19">
+        <v>51</v>
+      </c>
+      <c r="D19">
         <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19">
-        <v>50</v>
-      </c>
-      <c r="D19">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C20">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D20">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="C21">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D21">
         <v>7</v>
@@ -928,55 +922,55 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C22">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C23">
-        <v>60</v>
+        <v>98</v>
       </c>
       <c r="D23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>62</v>
+        <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="D24">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C25">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D25">
         <v>8</v>
@@ -984,97 +978,97 @@
     </row>
     <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C26">
         <v>99</v>
       </c>
       <c r="D26">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C27">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="C28">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D28">
-        <v>8.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D29">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D30">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C31">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C32">
-        <v>110</v>
+        <v>199</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -1082,239 +1076,217 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C33">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>22</v>
       </c>
       <c r="C34">
-        <v>199</v>
+        <v>999</v>
       </c>
       <c r="D34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B35" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="C35">
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C36">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>6</v>
+      <c r="A37" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
-      </c>
-      <c r="C37">
-        <v>1000</v>
-      </c>
-      <c r="D37">
-        <v>7</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>24</v>
-      </c>
-      <c r="C38">
-        <v>1000</v>
-      </c>
-      <c r="D38">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>37</v>
+      <c r="A50" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>38</v>
+      <c r="A51" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>40</v>
+      <c r="A55" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>47</v>
-      </c>
+      <c r="E56" s="2"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" t="s">
-        <v>47</v>
-      </c>
+      <c r="E57" s="2"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
@@ -1333,12 +1305,6 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
added "no soap here" message for T13
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{975AF580-03A4-4CFE-9275-763FEABEDE15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0A0EE9-8CF3-4A68-8201-766C30940BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t>Description</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>metahouse outside (only front site of house visible, everything else is cut off by black planes, trashcans should be visible (for T10))</t>
-  </si>
-  <si>
-    <t>H8 -&gt; "No soap here" when trying to wash hands downstairs</t>
   </si>
   <si>
     <t>when starting game for the first time -&gt; brightness slider ("move the slider so that the logo is barely visible")</t>
@@ -325,10 +322,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E55" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E55">
-    <sortCondition ref="C2:C55"/>
-    <sortCondition ref="D2:D55"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E54" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E54">
+    <sortCondition ref="C2:C54"/>
+    <sortCondition ref="D2:D54"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -604,7 +601,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -634,12 +631,12 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
@@ -653,7 +650,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -662,54 +659,54 @@
         <v>20</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="C6">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -721,9 +718,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -735,18 +732,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="C9">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D9">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -754,21 +751,21 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>48</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="C11">
         <v>48</v>
@@ -779,16 +776,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C12">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,7 +793,7 @@
         <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13">
         <v>49</v>
@@ -807,35 +804,35 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>49</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -844,29 +841,32 @@
         <v>50</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <v>51</v>
+      </c>
+      <c r="D17">
         <v>7</v>
       </c>
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17">
-        <v>50</v>
-      </c>
-      <c r="D17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C18">
         <v>51</v>
@@ -874,125 +874,122 @@
       <c r="D18">
         <v>7</v>
       </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C19">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20">
         <v>60</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>98</v>
+      </c>
+      <c r="D22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C22">
-        <v>70</v>
-      </c>
-      <c r="D22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
       <c r="C23">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D23">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>99</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
         <v>48</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
       </c>
       <c r="C25">
         <v>99</v>
       </c>
       <c r="D25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="C26">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D26">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
@@ -1001,26 +998,26 @@
         <v>100</v>
       </c>
       <c r="D27">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C28">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D28">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
@@ -1029,82 +1026,82 @@
         <v>110</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
         <v>23</v>
       </c>
       <c r="C30">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C31">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D31">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C32">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D32">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="C33">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>5</v>
+      <c r="A34" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B34" t="s">
         <v>22</v>
       </c>
       <c r="C34">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>6</v>
+      <c r="A35" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B35" t="s">
         <v>22</v>
@@ -1113,77 +1110,71 @@
         <v>1000</v>
       </c>
       <c r="D35">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C36">
-        <v>1000</v>
-      </c>
-      <c r="D36">
-        <v>9</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>68</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1191,47 +1182,47 @@
         <v>31</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>36</v>
+      <c r="A49" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1239,48 +1230,43 @@
         <v>42</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>53</v>
+      <c r="A54" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" t="s">
-        <v>45</v>
-      </c>
+      <c r="E55" s="2"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E56" s="2"/>
@@ -1302,9 +1288,6 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E63" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
improved flesh-food horror events
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0A0EE9-8CF3-4A68-8201-766C30940BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB1D0A1-E267-440D-8905-76311A47F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4695" yWindow="3390" windowWidth="26550" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -73,12 +73,6 @@
     <t>oven save within task</t>
   </si>
   <si>
-    <t>dialogue variation in food task</t>
-  </si>
-  <si>
-    <t>fleshplate doesn't fall down perfectly</t>
-  </si>
-  <si>
     <t>last food too late horror event</t>
   </si>
   <si>
@@ -208,9 +202,6 @@
     <t>water bottle, more glasses in the kitchen</t>
   </si>
   <si>
-    <t>H10 + H15 Flesh Plate: Flesh SFX, small glitch effect with the glitch sound</t>
-  </si>
-  <si>
     <t>H16 Puppet: SFX</t>
   </si>
   <si>
@@ -239,6 +230,9 @@
   </si>
   <si>
     <t>spieler nicht vom pc ausschließen (tasks dafür auch anpassen -&gt; wenn man die vernachlässigt, sollen neue horror events den spieler zuerst nerven, dann töten)</t>
+  </si>
+  <si>
+    <t>man ist selber im ofen und wird verbrannt</t>
   </si>
 </sst>
 </file>
@@ -322,10 +316,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E54" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E54">
-    <sortCondition ref="C2:C54"/>
-    <sortCondition ref="D2:D54"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E51" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
+    <sortCondition ref="C2:C51"/>
+    <sortCondition ref="D2:D51"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -601,7 +595,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -628,21 +622,21 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -650,139 +644,142 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C5">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5">
-        <v>33</v>
-      </c>
       <c r="D5">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C6">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C8">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D8">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C10">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="C11">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -790,480 +787,447 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="C15">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
         <v>22</v>
       </c>
-      <c r="C16">
-        <v>50</v>
-      </c>
-      <c r="D16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
       <c r="C17">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>7</v>
       </c>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C18">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19">
+        <v>98</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>99</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>99</v>
+      </c>
+      <c r="D21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>99</v>
+      </c>
+      <c r="D22">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19">
-        <v>60</v>
-      </c>
-      <c r="D19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20">
-        <v>60</v>
-      </c>
-      <c r="D20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21">
-        <v>70</v>
-      </c>
-      <c r="D21">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>98</v>
-      </c>
-      <c r="D22">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23">
-        <v>99</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="C24">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D24">
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C25">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D25">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D26">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C27">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D27">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28">
+        <v>199</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29">
+        <v>200</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30">
+        <v>999</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <v>1000</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32">
+        <v>1000</v>
+      </c>
+      <c r="D32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28">
-        <v>110</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
-      </c>
-      <c r="C29">
-        <v>110</v>
-      </c>
-      <c r="D29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B40" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30">
-        <v>120</v>
-      </c>
-      <c r="D30">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31">
-        <v>199</v>
-      </c>
-      <c r="D31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32">
-        <v>200</v>
-      </c>
-      <c r="D32">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33">
-        <v>999</v>
-      </c>
-      <c r="D33">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34">
-        <v>1000</v>
-      </c>
-      <c r="D34">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" t="s">
-        <v>22</v>
-      </c>
-      <c r="C35">
-        <v>1000</v>
-      </c>
-      <c r="D35">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B43" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B45" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="B48" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
-        <v>45</v>
+      <c r="A51" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" t="s">
-        <v>44</v>
-      </c>
+      <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" t="s">
-        <v>44</v>
-      </c>
+      <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" t="s">
-        <v>44</v>
-      </c>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E55" s="2"/>
@@ -1279,15 +1243,6 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E62" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
added many props and materials to the kitchen
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB1D0A1-E267-440D-8905-76311A47F960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667EEA0F-EC44-47F2-B5F1-5D19CDD09B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="3390" windowWidth="26550" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>Description</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Goblin in meta wegglitchen</t>
   </si>
   <si>
-    <t>Glas und Fensterscherben aufräumen müssen als task</t>
-  </si>
-  <si>
     <t>The glitch zwingt einem, zu spielen. Wenn man zu lange vom PC weg ist, wird man von ihm bestraft</t>
   </si>
   <si>
@@ -199,9 +196,6 @@
     <t>H9: more dialogue?</t>
   </si>
   <si>
-    <t>water bottle, more glasses in the kitchen</t>
-  </si>
-  <si>
     <t>H16 Puppet: SFX</t>
   </si>
   <si>
@@ -233,6 +227,12 @@
   </si>
   <si>
     <t>man ist selber im ofen und wird verbrannt</t>
+  </si>
+  <si>
+    <t>Glas und Fensterscherben aufräumen müssen als task?</t>
+  </si>
+  <si>
+    <t>Should it really?</t>
   </si>
 </sst>
 </file>
@@ -316,10 +316,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E51" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
-    <sortCondition ref="C2:C51"/>
-    <sortCondition ref="D2:D51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E50" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
+    <sortCondition ref="C2:C50"/>
+    <sortCondition ref="D2:D50"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -595,11 +595,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,40 +625,46 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -669,22 +675,19 @@
       <c r="D4">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -692,21 +695,21 @@
         <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>48</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C7">
         <v>48</v>
@@ -717,24 +720,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>49</v>
@@ -745,35 +748,35 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>49</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>20</v>
       </c>
       <c r="C11">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
@@ -782,29 +785,32 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>51</v>
+      </c>
+      <c r="D13">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>50</v>
-      </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C14">
         <v>51</v>
@@ -812,125 +818,122 @@
       <c r="D14">
         <v>7</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15">
         <v>60</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15">
-        <v>51</v>
-      </c>
       <c r="D15">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>60</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18">
+        <v>98</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C18">
-        <v>70</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
       <c r="C19">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>99</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
         <v>45</v>
-      </c>
-      <c r="B21" t="s">
-        <v>46</v>
       </c>
       <c r="C21">
         <v>99</v>
       </c>
       <c r="D21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D22">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>20</v>
@@ -939,26 +942,26 @@
         <v>100</v>
       </c>
       <c r="D23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
@@ -967,82 +970,82 @@
         <v>110</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
       </c>
       <c r="C26">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="C27">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C28">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="C29">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>5</v>
+      <c r="A30" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
       </c>
       <c r="C30">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>6</v>
+      <c r="A31" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B31" t="s">
         <v>20</v>
@@ -1051,125 +1054,119 @@
         <v>1000</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32">
-        <v>1000</v>
-      </c>
-      <c r="D32">
-        <v>9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>31</v>
+      <c r="A43" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>32</v>
+      <c r="A44" s="4" t="s">
+        <v>33</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>33</v>
+      <c r="A45" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B45" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1177,48 +1174,43 @@
         <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>50</v>
+      <c r="A50" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B51" t="s">
-        <v>42</v>
-      </c>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
@@ -1240,9 +1232,6 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
fixed save system and added last food horror event
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667EEA0F-EC44-47F2-B5F1-5D19CDD09B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B316941D-7707-4117-8797-EE21CEFB84EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="3390" windowWidth="26550" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -73,9 +73,6 @@
     <t>oven save within task</t>
   </si>
   <si>
-    <t>last food too late horror event</t>
-  </si>
-  <si>
     <t>'random rocks, fallen trees on green grass '</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>"Hello?", "Who's there?", "Weird"</t>
-  </si>
-  <si>
     <t>even more quests</t>
   </si>
   <si>
@@ -226,21 +220,35 @@
     <t>spieler nicht vom pc ausschließen (tasks dafür auch anpassen -&gt; wenn man die vernachlässigt, sollen neue horror events den spieler zuerst nerven, dann töten)</t>
   </si>
   <si>
-    <t>man ist selber im ofen und wird verbrannt</t>
-  </si>
-  <si>
     <t>Glas und Fensterscherben aufräumen müssen als task?</t>
   </si>
   <si>
     <t>Should it really?</t>
+  </si>
+  <si>
+    <t>"Hello?", "Who's there?", "Weird", "Wrong number I hope..."</t>
+  </si>
+  <si>
+    <t>Licht fixen!</t>
+  </si>
+  <si>
+    <t>improve last food too late horror event</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -277,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -289,18 +297,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -316,13 +327,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E50" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
-    <sortCondition ref="C2:C50"/>
-    <sortCondition ref="D2:D50"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E51" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
+    <sortCondition ref="C3:C51"/>
+    <sortCondition ref="D3:D51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{FE0B1C3C-98C3-4A53-BB36-B09B8B6E281C}" name="Type"/>
     <tableColumn id="3" xr3:uid="{5DD8EB09-8914-40D5-924D-451D2B02BA4C}" name="Priority"/>
     <tableColumn id="4" xr3:uid="{E0C4F60E-BEC0-48F5-8017-79F3081EDA3C}" name="Est. Workload (0-10)"/>
@@ -595,11 +606,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,94 +633,79 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
-        <v>46</v>
-      </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
         <v>33</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3">
-        <v>40</v>
-      </c>
-      <c r="D3">
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5">
         <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4">
-        <v>40</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C5">
-        <v>48</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>48</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>48</v>
@@ -720,24 +716,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C8">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C9">
         <v>49</v>
@@ -748,69 +744,66 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>49</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12">
         <v>50</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13">
-        <v>51</v>
-      </c>
       <c r="D13">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <v>51</v>
@@ -818,89 +811,92 @@
       <c r="D14">
         <v>7</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D15">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>60</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
       </c>
       <c r="C17">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="D18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
       <c r="C19">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="C20">
         <v>99</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -908,309 +904,320 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>99</v>
       </c>
       <c r="D21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>99</v>
+      </c>
+      <c r="D22">
         <v>8.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22">
-        <v>100</v>
-      </c>
-      <c r="D22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C23">
         <v>100</v>
       </c>
       <c r="D23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>100</v>
+      </c>
+      <c r="D24">
         <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24">
-        <v>110</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C25">
         <v>110</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C26">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="D26">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="C27">
-        <v>199</v>
+        <v>120</v>
       </c>
       <c r="D27">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C28">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29">
+        <v>200</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" t="s">
-        <v>20</v>
-      </c>
-      <c r="C29">
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30">
         <v>999</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30">
-        <v>1000</v>
-      </c>
-      <c r="D30">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C31">
         <v>1000</v>
       </c>
       <c r="D31">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>19</v>
+      </c>
+      <c r="C32">
+        <v>1000</v>
+      </c>
+      <c r="D32">
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="B34" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B40" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
-        <v>52</v>
+      <c r="A50" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E51" s="2"/>
+      <c r="A51" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
@@ -1233,9 +1240,12 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
     </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="2"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Unclear">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Unclear">
       <formula>NOT(ISERROR(SEARCH("Unclear",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fixed lighting (I think?)
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B316941D-7707-4117-8797-EE21CEFB84EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC6679E-7EB8-41EC-B543-B8E06A6ADC03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4695" yWindow="3390" windowWidth="26550" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="65">
   <si>
     <t>Description</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>"Hello?", "Who's there?", "Weird", "Wrong number I hope..."</t>
-  </si>
-  <si>
-    <t>Licht fixen!</t>
   </si>
   <si>
     <t>improve last food too late horror event</t>
@@ -306,12 +303,12 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -327,13 +324,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E51" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E51">
-    <sortCondition ref="C3:C51"/>
-    <sortCondition ref="D3:D51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E50" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E50">
+    <sortCondition ref="C2:C50"/>
+    <sortCondition ref="D2:D50"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{FE0B1C3C-98C3-4A53-BB36-B09B8B6E281C}" name="Type"/>
     <tableColumn id="3" xr3:uid="{5DD8EB09-8914-40D5-924D-451D2B02BA4C}" name="Priority"/>
     <tableColumn id="4" xr3:uid="{E0C4F60E-BEC0-48F5-8017-79F3081EDA3C}" name="Est. Workload (0-10)"/>
@@ -606,7 +603,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -640,72 +637,78 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2">
+        <v>33</v>
+      </c>
+      <c r="D2">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>61</v>
-      </c>
       <c r="B3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3">
-        <v>33</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C5">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D5">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>48</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>48</v>
@@ -716,21 +719,21 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
         <v>44</v>
@@ -744,35 +747,35 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C10">
         <v>49</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -781,29 +784,32 @@
         <v>50</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>51</v>
+      </c>
+      <c r="D13">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
+      <c r="E13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C14">
         <v>51</v>
@@ -811,97 +817,94 @@
       <c r="D14">
         <v>7</v>
       </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C15">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C16">
         <v>60</v>
       </c>
       <c r="D16">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D17">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>98</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
-        <v>70</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
       <c r="C19">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D19">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C20">
         <v>99</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>44</v>
@@ -910,26 +913,26 @@
         <v>99</v>
       </c>
       <c r="D21">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C22">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D22">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -938,26 +941,26 @@
         <v>100</v>
       </c>
       <c r="D23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
@@ -966,82 +969,82 @@
         <v>110</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
       </c>
       <c r="C26">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="C27">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D27">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="C28">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C29">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D29">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>5</v>
+      <c r="A30" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B30" t="s">
         <v>19</v>
       </c>
       <c r="C30">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>6</v>
+      <c r="A31" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B31" t="s">
         <v>19</v>
@@ -1050,42 +1053,36 @@
         <v>1000</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32">
-        <v>1000</v>
-      </c>
-      <c r="D32">
-        <v>9</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>9</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
         <v>40</v>
@@ -1093,15 +1090,15 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
@@ -1109,7 +1106,7 @@
     </row>
     <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B38" t="s">
         <v>40</v>
@@ -1117,7 +1114,7 @@
     </row>
     <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
         <v>40</v>
@@ -1125,47 +1122,47 @@
     </row>
     <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B40" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>30</v>
+      <c r="A43" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B43" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>31</v>
+      <c r="A44" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B44" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>32</v>
+      <c r="A45" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
@@ -1173,7 +1170,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
@@ -1181,7 +1178,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B47" t="s">
         <v>40</v>
@@ -1189,7 +1186,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
@@ -1197,27 +1194,22 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>48</v>
+      <c r="A50" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="B50" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B51" t="s">
-        <v>40</v>
-      </c>
+      <c r="E51" s="2"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
@@ -1240,12 +1232,9 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E58" s="2"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E59" s="2"/>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Unclear">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Unclear">
       <formula>NOT(ISERROR(SEARCH("Unclear",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
improved h16; added sounds to T10; added knife materials
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6735F29-D52F-429F-8249-60C82E52C23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9B0BD6-5CB2-4404-9AA0-6E1FE1B158E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Gameplay Addition</t>
   </si>
   <si>
-    <t>Wall Texture (Wallpapers?)</t>
-  </si>
-  <si>
     <t>metahouse outside (only front site of house visible, everything else is cut off by black planes, trashcans should be visible (for T10))</t>
   </si>
   <si>
@@ -175,12 +172,6 @@
     <t>Small Change</t>
   </si>
   <si>
-    <t>T10 Trash SFX</t>
-  </si>
-  <si>
-    <t>knife materials, trail</t>
-  </si>
-  <si>
     <t>T13 Wash Hands: Better reason</t>
   </si>
   <si>
@@ -193,16 +184,10 @@
     <t>H9: more dialogue?</t>
   </si>
   <si>
-    <t>H16 Puppet: SFX</t>
-  </si>
-  <si>
     <t>H16 Puppet: better DestroyWhenNotLooking?</t>
   </si>
   <si>
     <t>Fun</t>
-  </si>
-  <si>
-    <t>QoL, Audio Only</t>
   </si>
   <si>
     <t>Notes</t>
@@ -321,10 +306,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E49" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E49">
-    <sortCondition ref="C2:C49"/>
-    <sortCondition ref="D2:D49"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E45" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E45">
+    <sortCondition ref="C2:C45"/>
+    <sortCondition ref="D2:D45"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -600,11 +585,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E57"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,15 +615,15 @@
         <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -647,127 +632,130 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C4">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C9">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>60</v>
+      </c>
+      <c r="D11">
         <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11">
-        <v>50</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -778,442 +766,383 @@
         <v>20</v>
       </c>
       <c r="C12">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D12">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C14">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="D14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="C15">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="D15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C16">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C17">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C18">
-        <v>99</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B19" t="s">
-        <v>44</v>
-      </c>
       <c r="C19">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C20">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="D20">
-        <v>8.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C22">
-        <v>100</v>
+        <v>199</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C23">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C24">
-        <v>110</v>
+        <v>999</v>
       </c>
       <c r="D24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="B25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C25">
-        <v>120</v>
+        <v>1000</v>
       </c>
       <c r="D25">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="C26">
-        <v>199</v>
+        <v>1000</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27">
-        <v>200</v>
-      </c>
-      <c r="D27">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28">
-        <v>999</v>
-      </c>
-      <c r="D28">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>6</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29">
-        <v>1000</v>
-      </c>
-      <c r="D29">
-        <v>7</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30">
-        <v>1000</v>
-      </c>
-      <c r="D30">
-        <v>9</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B36" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="B42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>32</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B48" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E50" s="2"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E51" s="2"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E57" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
added fallen logs and rocks to the field
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9B0BD6-5CB2-4404-9AA0-6E1FE1B158E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07688D60-1E1F-41EA-B734-83B90CF13167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
   <si>
     <t>Description</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>oven save within task</t>
-  </si>
-  <si>
-    <t>'random rocks, fallen trees on green grass '</t>
   </si>
   <si>
     <t>typisches leichtes bassiges beben</t>
@@ -306,10 +303,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E45" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E45">
-    <sortCondition ref="C2:C45"/>
-    <sortCondition ref="D2:D45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E44" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E44">
+    <sortCondition ref="C2:C44"/>
+    <sortCondition ref="D2:D44"/>
   </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
@@ -585,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -612,18 +609,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -632,23 +629,23 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>49</v>
@@ -659,10 +656,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5">
         <v>49</v>
@@ -673,38 +670,41 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
       <c r="C7">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>51</v>
@@ -712,300 +712,291 @@
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C9">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>60</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D11">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D13">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>99</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
         <v>42</v>
-      </c>
-      <c r="B15" t="s">
-        <v>43</v>
       </c>
       <c r="C15">
         <v>99</v>
       </c>
       <c r="D15">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="C16">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D16">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>100</v>
       </c>
       <c r="D17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D18">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19">
         <v>110</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C20">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="C21">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D21">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>53</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C22">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D22">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="C23">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
+      <c r="A24" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C24">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>6</v>
+      <c r="A25" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C25">
         <v>1000</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26">
-        <v>1000</v>
-      </c>
-      <c r="D26">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1013,15 +1004,15 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1029,47 +1020,47 @@
         <v>26</v>
       </c>
       <c r="B34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>31</v>
+      <c r="A39" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1077,48 +1068,43 @@
         <v>36</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>45</v>
+      <c r="A44" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" t="s">
-        <v>39</v>
-      </c>
+      <c r="E45" s="2"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E46" s="2"/>
@@ -1140,9 +1126,6 @@
     </row>
     <row r="52" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E53" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>

<commit_message>
added many new models and textures/materials
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07688D60-1E1F-41EA-B734-83B90CF13167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1492054-D5BD-4672-A4B9-0B156154D840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,9 +58,6 @@
     <t>better mountains</t>
   </si>
   <si>
-    <t>better meta models</t>
-  </si>
-  <si>
     <t>reminder of current task when doing nothing for too long</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>somehow improve last food too late horror event</t>
+  </si>
+  <si>
+    <t>better lamps: add materials and swap material to a glowing one when on</t>
   </si>
 </sst>
 </file>
@@ -282,12 +282,12 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FFFF0000"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -309,7 +309,7 @@
     <sortCondition ref="D2:D44"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{FE0B1C3C-98C3-4A53-BB36-B09B8B6E281C}" name="Type"/>
     <tableColumn id="3" xr3:uid="{5DD8EB09-8914-40D5-924D-451D2B02BA4C}" name="Priority"/>
     <tableColumn id="4" xr3:uid="{E0C4F60E-BEC0-48F5-8017-79F3081EDA3C}" name="Est. Workload (0-10)"/>
@@ -586,7 +586,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,18 +609,18 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>33</v>
@@ -629,15 +629,21 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="C3">
+        <v>49</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -645,7 +651,7 @@
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>49</v>
@@ -656,58 +662,58 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6">
+        <v>51</v>
+      </c>
+      <c r="D6">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-      <c r="D6">
-        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C7">
-        <v>51</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
       <c r="C8">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="D8">
         <v>7</v>
@@ -715,392 +721,386 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="D11">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C12">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D12">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C13">
         <v>99</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
         <v>41</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
       </c>
       <c r="C14">
         <v>99</v>
       </c>
       <c r="D14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D15">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>100</v>
       </c>
       <c r="D16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D17">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18">
         <v>110</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="D19">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="C20">
-        <v>120</v>
+        <v>199</v>
       </c>
       <c r="D20">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C21">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="C22">
-        <v>200</v>
+        <v>999</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
+      <c r="A23" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>6</v>
+      <c r="A24" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>1000</v>
       </c>
       <c r="D24">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25">
-        <v>1000</v>
-      </c>
-      <c r="D25">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1129,7 +1129,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Unclear">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Unclear">
       <formula>NOT(ISERROR(SEARCH("Unclear",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
multiple smaller improvements and fixes
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6C4BF9-40C6-42E3-B0B0-DF050E2B6F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17410124-7B2A-4F21-8E38-7D705AF59413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
   <si>
     <t>Description</t>
   </si>
@@ -49,66 +49,30 @@
     <t>castle interiors (throne room)</t>
   </si>
   <si>
-    <t>add fake other players (manu and fish)</t>
-  </si>
-  <si>
-    <t>more npc variants</t>
-  </si>
-  <si>
     <t>better mountains</t>
   </si>
   <si>
-    <t>reminder of current task when doing nothing for too long</t>
-  </si>
-  <si>
-    <t>change time on clock after important events</t>
-  </si>
-  <si>
-    <t>more horror during food task</t>
-  </si>
-  <si>
     <t>oven save within task</t>
   </si>
   <si>
-    <t>typisches leichtes bassiges beben</t>
-  </si>
-  <si>
     <t>put minigames here and there, e.g. a gameboy with tetris</t>
   </si>
   <si>
     <t>?? TankBattlePremium Experimental 2 Ending instead of/after current ending</t>
   </si>
   <si>
-    <t>instead of forcing the player to do all tasks sequentially, give him a list of things to do (maybe event do it so that the player isn't blocked from playing)</t>
-  </si>
-  <si>
     <t>washing machine beep -&gt; hear it inGame; don't block player from playing while waiting, maybe increase time</t>
   </si>
   <si>
     <t>Est. Workload (0-10)</t>
   </si>
   <si>
-    <t>QoL, Visual Only</t>
-  </si>
-  <si>
-    <t>QoL</t>
-  </si>
-  <si>
-    <t>Gameplay Addition</t>
-  </si>
-  <si>
-    <t>metahouse outside (only front site of house visible, everything else is cut off by black planes, trashcans should be visible (for T10))</t>
-  </si>
-  <si>
     <t>when starting game for the first time -&gt; brightness slider ("move the slider so that the logo is barely visible")</t>
   </si>
   <si>
     <t>T8 cracker save state of the optional cola bottle</t>
   </si>
   <si>
-    <t>QoL, SFX Addition</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mutter ruft am Anfang an und sagt, man solle die Tasks machen, die auf einem Zettel stehen, bevor die morgen früh wieder kommt </t>
   </si>
   <si>
@@ -130,21 +94,12 @@
     <t xml:space="preserve">Wäsche zusammenlegen quest </t>
   </si>
   <si>
-    <t>The glitch und andere glitches in game haben</t>
-  </si>
-  <si>
     <t>The glitch zwingt einem, zu spielen. Wenn man zu lange vom PC weg ist, wird man von ihm bestraft</t>
   </si>
   <si>
     <t>Game over wenn man im Spiel zu langsam voran kommt</t>
   </si>
   <si>
-    <t xml:space="preserve">Knopf für Steuerung im Menü mit rebinding? </t>
-  </si>
-  <si>
-    <t>Unclear</t>
-  </si>
-  <si>
     <t>man wird nur ins spiel gezogen, wenn man zu viel spielt</t>
   </si>
   <si>
@@ -154,24 +109,6 @@
     <t>Passanten vor Fenstern vorbeilaufen bzw. Horror Event where you see someone walking away from the window</t>
   </si>
   <si>
-    <t>Horror</t>
-  </si>
-  <si>
-    <t>Small Change</t>
-  </si>
-  <si>
-    <t>T13 Wash Hands: Better reason</t>
-  </si>
-  <si>
-    <t>H9: more dialogue?</t>
-  </si>
-  <si>
-    <t>H16 Puppet: better DestroyWhenNotLooking?</t>
-  </si>
-  <si>
-    <t>Fun</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -187,13 +124,34 @@
     <t>Glas und Fensterscherben aufräumen müssen als task?</t>
   </si>
   <si>
-    <t>Should it really?</t>
-  </si>
-  <si>
-    <t>somehow improve last food too late horror event</t>
-  </si>
-  <si>
-    <t>better lamps: add materials and swap material to a glowing one when on</t>
+    <t>add manu and fish as npcs</t>
+  </si>
+  <si>
+    <t>remind player when doing no tasks for too long</t>
+  </si>
+  <si>
+    <t>Unlikely</t>
+  </si>
+  <si>
+    <t>typisches leichtes bassiges beben here and there</t>
+  </si>
+  <si>
+    <t>Seperation</t>
+  </si>
+  <si>
+    <t>instead of forcing the player to do all tasks sequentially, give him a list of things to do</t>
+  </si>
+  <si>
+    <t>really slow tts: "PLAY THE GAME"</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>NextNext</t>
+  </si>
+  <si>
+    <t>NextNextNext</t>
   </si>
 </sst>
 </file>
@@ -209,7 +167,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -246,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -261,11 +219,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -288,13 +269,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E40" totalsRowShown="0">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E40">
-    <sortCondition ref="C2:C40"/>
-    <sortCondition ref="D2:D40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{959E9826-352F-41AC-AD9F-03752DFFD7FE}" name="Tabelle1" displayName="Tabelle1" ref="A1:E29" totalsRowShown="0">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E29">
+    <sortCondition ref="B2:B29"/>
+    <sortCondition ref="D2:D29"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FE8F8640-C33C-4C90-855D-705C4F08A50D}" name="Description" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{FE0B1C3C-98C3-4A53-BB36-B09B8B6E281C}" name="Type"/>
     <tableColumn id="3" xr3:uid="{5DD8EB09-8914-40D5-924D-451D2B02BA4C}" name="Priority"/>
     <tableColumn id="4" xr3:uid="{E0C4F60E-BEC0-48F5-8017-79F3081EDA3C}" name="Est. Workload (0-10)"/>
@@ -567,20 +548,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="94.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="96.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -594,38 +576,29 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>49</v>
+      <c r="A2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -633,69 +606,54 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="D5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>80</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
+      <c r="A8" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -703,360 +661,286 @@
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="D9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="D10">
-        <v>8.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>100</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>100</v>
-      </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13">
-        <v>110</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>10</v>
+      <c r="A14" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>110</v>
+        <v>33</v>
       </c>
       <c r="D14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16">
-        <v>199</v>
+        <v>33</v>
       </c>
       <c r="D16">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>12</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17">
-        <v>200</v>
+        <v>33</v>
       </c>
       <c r="D17">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18">
-        <v>999</v>
+        <v>33</v>
       </c>
       <c r="D18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19">
-        <v>1000</v>
+        <v>33</v>
       </c>
       <c r="D19">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20">
-        <v>1000</v>
-      </c>
-      <c r="D20">
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E48" s="2"/>
+      <c r="D29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Unclear">
+      <formula>NOT(ISERROR(SEARCH("Unclear",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Unclear">
+      <formula>NOT(ISERROR(SEARCH("Unclear",B17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Unclear">
+      <formula>NOT(ISERROR(SEARCH("Unclear",E26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Unclear">
+      <formula>NOT(ISERROR(SEARCH("Unclear",E29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Unclear">
-      <formula>NOT(ISERROR(SEARCH("Unclear",B1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Unclear",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
many bugfixes and some small improvements
</commit_message>
<xml_diff>
--- a/Documents/TODO.xlsx
+++ b/Documents/TODO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\User\GameEngines\Unity\isekai-fake-rpg\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A86344-038F-4058-9839-E3D6AE27DEA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99CD8A1A-6EE7-4B1E-A9A7-D71BF535C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="1695" windowWidth="26550" windowHeight="15255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -540,11 +540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,24 +822,28 @@
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E26" s="2"/>
+      <c r="A26"/>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E27" s="2"/>
+      <c r="A27"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E29" s="2"/>
+      <c r="A28"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E30" s="2"/>
+      <c r="A30"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B25 B33:B1048576 A31 A28">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Unclear">
-      <formula>NOT(ISERROR(SEARCH("Unclear",B1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Unclear",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">

</xml_diff>